<commit_message>
Actualizado excel y añadido GDD, me falta rellenar algunas cosillas del GDD con imagenes pero la base ya  está.
</commit_message>
<xml_diff>
--- a/Sprint-1_Mecanicas.xlsx
+++ b/Sprint-1_Mecanicas.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI-D\Documents\MecanicasAvanzao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iriag\Desktop\Alex\Definetly_Not_Pong\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8FCA27-3FA8-4477-8404-4DBE4AC2CF3D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="68">
   <si>
     <t>Subtarea</t>
   </si>
@@ -230,7 +231,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -342,7 +343,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,12 +404,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="38">
     <border>
@@ -1230,6 +1225,42 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1273,15 +1304,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1293,17 +1315,11 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1317,6 +1333,15 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1350,37 +1375,7 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1403,7 +1398,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1498,13 +1493,13 @@
                   <c:v>16.676600000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.676600000000001</c:v>
+                  <c:v>15.676600000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.676600000000001</c:v>
+                  <c:v>15.676600000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.676600000000001</c:v>
+                  <c:v>15.676600000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1588,7 +1583,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1683,13 +1678,13 @@
                   <c:v>16.676600000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.676600000000001</c:v>
+                  <c:v>15.676600000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.676600000000001</c:v>
+                  <c:v>15.676600000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.676600000000001</c:v>
+                  <c:v>15.676600000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1855,7 +1850,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2174,58 +2169,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="N27" sqref="N27:N30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="43.6640625" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" customWidth="1"/>
-    <col min="4" max="4" width="55.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" customWidth="1"/>
-    <col min="15" max="15" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
+    <col min="4" max="4" width="55.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="46.8" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="1" spans="1:37" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A1" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="131" t="s">
+      <c r="C1" s="115" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
-    </row>
-    <row r="2" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J2" s="110" t="s">
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+    </row>
+    <row r="2" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="112"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
+      <c r="Q2" s="124"/>
       <c r="R2" s="52"/>
       <c r="S2" s="42"/>
       <c r="T2" s="42"/>
@@ -2247,7 +2242,7 @@
       <c r="AJ2" s="42"/>
       <c r="AK2" s="42"/>
     </row>
-    <row r="3" spans="1:37" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
@@ -2317,8 +2312,8 @@
       <c r="AJ3" s="41"/>
       <c r="AK3" s="41"/>
     </row>
-    <row r="4" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="113" t="s">
+    <row r="4" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="125" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="82" t="s">
@@ -2353,7 +2348,7 @@
       <c r="M4" s="106">
         <v>0</v>
       </c>
-      <c r="N4" s="155">
+      <c r="N4" s="110">
         <v>0</v>
       </c>
       <c r="O4" s="24"/>
@@ -2380,8 +2375,8 @@
       <c r="AJ4" s="25"/>
       <c r="AK4" s="25"/>
     </row>
-    <row r="5" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="114"/>
+    <row r="5" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="126"/>
       <c r="C5" s="85" t="s">
         <v>31</v>
       </c>
@@ -2414,7 +2409,7 @@
       <c r="M5" s="106">
         <v>0</v>
       </c>
-      <c r="N5" s="156">
+      <c r="N5" s="111">
         <v>0.11700000000000001</v>
       </c>
       <c r="O5" s="25"/>
@@ -2441,8 +2436,8 @@
       <c r="AJ5" s="25"/>
       <c r="AK5" s="25"/>
     </row>
-    <row r="6" spans="1:37" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="114"/>
+    <row r="6" spans="1:37" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="126"/>
       <c r="C6" s="85" t="s">
         <v>30</v>
       </c>
@@ -2475,7 +2470,7 @@
       <c r="M6" s="106">
         <v>0</v>
       </c>
-      <c r="N6" s="157">
+      <c r="N6" s="160">
         <v>1.67E-2</v>
       </c>
       <c r="O6" s="25"/>
@@ -2502,8 +2497,8 @@
       <c r="AJ6" s="25"/>
       <c r="AK6" s="25"/>
     </row>
-    <row r="7" spans="1:37" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="115"/>
+    <row r="7" spans="1:37" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="127"/>
       <c r="C7" s="88" t="s">
         <v>32</v>
       </c>
@@ -2536,7 +2531,7 @@
       <c r="M7" s="106">
         <v>0</v>
       </c>
-      <c r="N7" s="158">
+      <c r="N7" s="112">
         <v>0</v>
       </c>
       <c r="O7" s="70"/>
@@ -2563,11 +2558,11 @@
       <c r="AJ7" s="25"/>
       <c r="AK7" s="37"/>
     </row>
-    <row r="8" spans="1:37" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="119" t="s">
+    <row r="8" spans="1:37" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="131" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="122" t="s">
+      <c r="C8" s="134" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="91" t="s">
@@ -2626,9 +2621,9 @@
       <c r="AJ8" s="25"/>
       <c r="AK8" s="25"/>
     </row>
-    <row r="9" spans="1:37" ht="23.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="120"/>
-      <c r="C9" s="123"/>
+    <row r="9" spans="1:37" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="132"/>
+      <c r="C9" s="135"/>
       <c r="D9" s="92" t="s">
         <v>59</v>
       </c>
@@ -2685,9 +2680,9 @@
       <c r="AJ9" s="25"/>
       <c r="AK9" s="25"/>
     </row>
-    <row r="10" spans="1:37" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="120"/>
-      <c r="C10" s="123"/>
+    <row r="10" spans="1:37" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="132"/>
+      <c r="C10" s="135"/>
       <c r="D10" s="92" t="s">
         <v>36</v>
       </c>
@@ -2744,9 +2739,9 @@
       <c r="AJ10" s="25"/>
       <c r="AK10" s="25"/>
     </row>
-    <row r="11" spans="1:37" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="121"/>
-      <c r="C11" s="124"/>
+    <row r="11" spans="1:37" ht="22.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="133"/>
+      <c r="C11" s="136"/>
       <c r="D11" s="93" t="s">
         <v>66</v>
       </c>
@@ -2803,7 +2798,7 @@
       <c r="AJ11" s="25"/>
       <c r="AK11" s="25"/>
     </row>
-    <row r="12" spans="1:37" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="94" t="s">
         <v>38</v>
       </c>
@@ -2825,7 +2820,7 @@
       </c>
       <c r="I12" s="9">
         <f t="shared" si="0"/>
-        <v>1.17</v>
+        <v>2.17</v>
       </c>
       <c r="J12" s="106">
         <v>0</v>
@@ -2842,7 +2837,9 @@
       <c r="N12" s="107">
         <v>0.5</v>
       </c>
-      <c r="O12" s="73"/>
+      <c r="O12" s="107">
+        <v>1</v>
+      </c>
       <c r="P12" s="73"/>
       <c r="Q12" s="75"/>
       <c r="R12" s="48"/>
@@ -2866,11 +2863,11 @@
       <c r="AJ12" s="25"/>
       <c r="AK12" s="25"/>
     </row>
-    <row r="13" spans="1:37" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="125" t="s">
+    <row r="13" spans="1:37" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="116" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="132" t="s">
+      <c r="C13" s="119" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="83" t="s">
@@ -2904,7 +2901,7 @@
       <c r="M13" s="108">
         <v>0</v>
       </c>
-      <c r="N13" s="159">
+      <c r="N13" s="113">
         <v>0.83299999999999996</v>
       </c>
       <c r="O13" s="24"/>
@@ -2931,9 +2928,9 @@
       <c r="AJ13" s="25"/>
       <c r="AK13" s="25"/>
     </row>
-    <row r="14" spans="1:37" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="126"/>
-      <c r="C14" s="133"/>
+    <row r="14" spans="1:37" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="117"/>
+      <c r="C14" s="120"/>
       <c r="D14" s="86" t="s">
         <v>65</v>
       </c>
@@ -2965,7 +2962,7 @@
       <c r="M14" s="108">
         <v>0</v>
       </c>
-      <c r="N14" s="160">
+      <c r="N14" s="114">
         <v>0</v>
       </c>
       <c r="O14" s="25"/>
@@ -2992,9 +2989,9 @@
       <c r="AJ14" s="25"/>
       <c r="AK14" s="25"/>
     </row>
-    <row r="15" spans="1:37" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="126"/>
-      <c r="C15" s="133"/>
+    <row r="15" spans="1:37" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="117"/>
+      <c r="C15" s="120"/>
       <c r="D15" s="99" t="s">
         <v>64</v>
       </c>
@@ -3026,7 +3023,7 @@
       <c r="M15" s="108">
         <v>0</v>
       </c>
-      <c r="N15" s="25">
+      <c r="N15" s="108">
         <v>0</v>
       </c>
       <c r="O15" s="25"/>
@@ -3053,9 +3050,9 @@
       <c r="AJ15" s="25"/>
       <c r="AK15" s="25"/>
     </row>
-    <row r="16" spans="1:37" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="126"/>
-      <c r="C16" s="133"/>
+    <row r="16" spans="1:37" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="117"/>
+      <c r="C16" s="120"/>
       <c r="D16" s="86" t="s">
         <v>61</v>
       </c>
@@ -3087,7 +3084,7 @@
       <c r="M16" s="108">
         <v>0</v>
       </c>
-      <c r="N16" s="156">
+      <c r="N16" s="111">
         <v>0.2</v>
       </c>
       <c r="O16" s="25"/>
@@ -3114,9 +3111,9 @@
       <c r="AJ16" s="37"/>
       <c r="AK16" s="25"/>
     </row>
-    <row r="17" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="126"/>
-      <c r="C17" s="133"/>
+    <row r="17" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="117"/>
+      <c r="C17" s="120"/>
       <c r="D17" s="86" t="s">
         <v>41</v>
       </c>
@@ -3148,7 +3145,7 @@
       <c r="M17" s="108">
         <v>0</v>
       </c>
-      <c r="N17" s="160">
+      <c r="N17" s="114">
         <v>0</v>
       </c>
       <c r="O17" s="25"/>
@@ -3175,9 +3172,9 @@
       <c r="AJ17" s="37"/>
       <c r="AK17" s="25"/>
     </row>
-    <row r="18" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="127"/>
-      <c r="C18" s="134"/>
+    <row r="18" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="118"/>
+      <c r="C18" s="121"/>
       <c r="D18" s="89" t="s">
         <v>48</v>
       </c>
@@ -3209,7 +3206,7 @@
       <c r="M18" s="108">
         <v>0</v>
       </c>
-      <c r="N18" s="158">
+      <c r="N18" s="112">
         <v>0</v>
       </c>
       <c r="O18" s="70"/>
@@ -3236,11 +3233,11 @@
       <c r="AJ18" s="37"/>
       <c r="AK18" s="25"/>
     </row>
-    <row r="19" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="125" t="s">
+    <row r="19" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="132" t="s">
+      <c r="C19" s="119" t="s">
         <v>35</v>
       </c>
       <c r="D19" s="83" t="s">
@@ -3274,7 +3271,7 @@
       <c r="M19" s="108">
         <v>0</v>
       </c>
-      <c r="N19" s="159">
+      <c r="N19" s="113">
         <v>1.67E-2</v>
       </c>
       <c r="O19" s="24"/>
@@ -3301,9 +3298,9 @@
       <c r="AJ19" s="37"/>
       <c r="AK19" s="25"/>
     </row>
-    <row r="20" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="126"/>
-      <c r="C20" s="133"/>
+    <row r="20" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="117"/>
+      <c r="C20" s="120"/>
       <c r="D20" s="92" t="s">
         <v>59</v>
       </c>
@@ -3362,9 +3359,9 @@
       <c r="AJ20" s="37"/>
       <c r="AK20" s="25"/>
     </row>
-    <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="126"/>
-      <c r="C21" s="133"/>
+    <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="117"/>
+      <c r="C21" s="120"/>
       <c r="D21" s="92" t="s">
         <v>60</v>
       </c>
@@ -3423,9 +3420,9 @@
       <c r="AJ21" s="37"/>
       <c r="AK21" s="25"/>
     </row>
-    <row r="22" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="127"/>
-      <c r="C22" s="134"/>
+    <row r="22" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="118"/>
+      <c r="C22" s="121"/>
       <c r="D22" s="93" t="s">
         <v>61</v>
       </c>
@@ -3484,8 +3481,8 @@
       <c r="AJ22" s="37"/>
       <c r="AK22" s="25"/>
     </row>
-    <row r="23" spans="2:37" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="125" t="s">
+    <row r="23" spans="2:37" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="116" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="97" t="s">
@@ -3520,7 +3517,7 @@
       <c r="M23" s="108">
         <v>0</v>
       </c>
-      <c r="N23" s="159">
+      <c r="N23" s="113">
         <v>0.02</v>
       </c>
       <c r="O23" s="24"/>
@@ -3547,8 +3544,8 @@
       <c r="AJ23" s="37"/>
       <c r="AK23" s="25"/>
     </row>
-    <row r="24" spans="2:37" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="126"/>
+    <row r="24" spans="2:37" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="117"/>
       <c r="C24" s="100" t="s">
         <v>54</v>
       </c>
@@ -3579,7 +3576,7 @@
       <c r="M24" s="108">
         <v>0</v>
       </c>
-      <c r="N24" s="25">
+      <c r="N24" s="108">
         <v>0</v>
       </c>
       <c r="O24" s="25"/>
@@ -3606,8 +3603,8 @@
       <c r="AJ24" s="37"/>
       <c r="AK24" s="25"/>
     </row>
-    <row r="25" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="126"/>
+    <row r="25" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="117"/>
       <c r="C25" s="101" t="s">
         <v>44</v>
       </c>
@@ -3638,7 +3635,7 @@
       <c r="M25" s="108">
         <v>0</v>
       </c>
-      <c r="N25" s="25">
+      <c r="N25" s="108">
         <v>0</v>
       </c>
       <c r="O25" s="25"/>
@@ -3665,8 +3662,8 @@
       <c r="AJ25" s="38"/>
       <c r="AK25" s="37"/>
     </row>
-    <row r="26" spans="2:37" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="127"/>
+    <row r="26" spans="2:37" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="118"/>
       <c r="C26" s="102" t="s">
         <v>53</v>
       </c>
@@ -3718,11 +3715,11 @@
       <c r="AJ26" s="37"/>
       <c r="AK26" s="37"/>
     </row>
-    <row r="27" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="125" t="s">
+    <row r="27" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="128" t="s">
+      <c r="C27" s="137" t="s">
         <v>35</v>
       </c>
       <c r="D27" s="91" t="s">
@@ -3781,9 +3778,9 @@
       <c r="AJ27" s="37"/>
       <c r="AK27" s="37"/>
     </row>
-    <row r="28" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="126"/>
-      <c r="C28" s="129"/>
+    <row r="28" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="117"/>
+      <c r="C28" s="138"/>
       <c r="D28" s="92" t="s">
         <v>67</v>
       </c>
@@ -3840,9 +3837,9 @@
       <c r="AJ28" s="37"/>
       <c r="AK28" s="37"/>
     </row>
-    <row r="29" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="126"/>
-      <c r="C29" s="129"/>
+    <row r="29" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="117"/>
+      <c r="C29" s="138"/>
       <c r="D29" s="92" t="s">
         <v>46</v>
       </c>
@@ -3899,9 +3896,9 @@
       <c r="AJ29" s="37"/>
       <c r="AK29" s="37"/>
     </row>
-    <row r="30" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="127"/>
-      <c r="C30" s="130"/>
+    <row r="30" spans="2:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="118"/>
+      <c r="C30" s="139"/>
       <c r="D30" s="93" t="s">
         <v>47</v>
       </c>
@@ -3958,22 +3955,22 @@
       <c r="AJ30" s="37"/>
       <c r="AK30" s="37"/>
     </row>
-    <row r="31" spans="2:37" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="117" t="s">
+    <row r="31" spans="2:37" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="118"/>
-      <c r="D31" s="118"/>
-      <c r="E31" s="118"/>
-      <c r="F31" s="118"/>
-      <c r="G31" s="118"/>
+      <c r="C31" s="130"/>
+      <c r="D31" s="130"/>
+      <c r="E31" s="130"/>
+      <c r="F31" s="130"/>
+      <c r="G31" s="130"/>
       <c r="H31" s="78">
         <f>SUM(H4:H30)</f>
         <v>19.8</v>
       </c>
       <c r="I31" s="78">
         <f>SUM(I4:I30)</f>
-        <v>3.1234000000000002</v>
+        <v>4.1234000000000002</v>
       </c>
       <c r="J31" s="78">
         <f>SUM(J4:J30)</f>
@@ -3997,7 +3994,7 @@
       </c>
       <c r="O31" s="78">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P31" s="78">
         <f t="shared" si="1"/>
@@ -4028,7 +4025,7 @@
       <c r="AJ31" s="35"/>
       <c r="AK31" s="35"/>
     </row>
-    <row r="32" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -4037,16 +4034,16 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="110" t="s">
+      <c r="J32" s="122" t="s">
         <v>11</v>
       </c>
-      <c r="K32" s="111"/>
-      <c r="L32" s="111"/>
-      <c r="M32" s="111"/>
-      <c r="N32" s="111"/>
-      <c r="O32" s="111"/>
-      <c r="P32" s="111"/>
-      <c r="Q32" s="116"/>
+      <c r="K32" s="123"/>
+      <c r="L32" s="123"/>
+      <c r="M32" s="123"/>
+      <c r="N32" s="123"/>
+      <c r="O32" s="123"/>
+      <c r="P32" s="123"/>
+      <c r="Q32" s="128"/>
       <c r="R32" s="42"/>
       <c r="S32" s="42"/>
       <c r="T32" s="42"/>
@@ -4068,7 +4065,7 @@
       <c r="AJ32" s="42"/>
       <c r="AK32" s="42"/>
     </row>
-    <row r="33" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="16" t="s">
         <v>19</v>
       </c>
@@ -4112,7 +4109,7 @@
       <c r="AJ33" s="45"/>
       <c r="AK33" s="45"/>
     </row>
-    <row r="34" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="79" t="s">
         <v>14</v>
       </c>
@@ -4130,10 +4127,10 @@
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="110" t="s">
+      <c r="H34" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="I34" s="116"/>
+      <c r="I34" s="128"/>
       <c r="J34" s="9">
         <f>SUM(H31,-J31)</f>
         <v>19.05</v>
@@ -4156,15 +4153,15 @@
       </c>
       <c r="O34" s="9">
         <f t="shared" si="2"/>
-        <v>16.676600000000001</v>
+        <v>15.676600000000001</v>
       </c>
       <c r="P34" s="9">
         <f t="shared" si="2"/>
-        <v>16.676600000000001</v>
+        <v>15.676600000000001</v>
       </c>
       <c r="Q34" s="9">
         <f t="shared" si="2"/>
-        <v>16.676600000000001</v>
+        <v>15.676600000000001</v>
       </c>
       <c r="R34" s="35"/>
       <c r="S34" s="35"/>
@@ -4187,7 +4184,7 @@
       <c r="AJ34" s="35"/>
       <c r="AK34" s="35"/>
     </row>
-    <row r="35" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="80" t="s">
         <v>13</v>
       </c>
@@ -4232,7 +4229,7 @@
       <c r="AJ35" s="45"/>
       <c r="AK35" s="45"/>
     </row>
-    <row r="36" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="81" t="s">
         <v>15</v>
       </c>
@@ -4242,28 +4239,28 @@
       </c>
       <c r="D36" s="31">
         <f>SUM(I12,I15,I24:I26)</f>
-        <v>1.92</v>
+        <v>2.92</v>
       </c>
       <c r="E36" s="29">
         <f t="shared" si="3"/>
-        <v>4.38</v>
+        <v>3.38</v>
       </c>
       <c r="F36" s="3"/>
-      <c r="H36" s="110" t="s">
+      <c r="H36" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="I36" s="111"/>
-      <c r="J36" s="110">
+      <c r="I36" s="123"/>
+      <c r="J36" s="122">
         <f>H31-I31</f>
-        <v>16.676600000000001</v>
-      </c>
-      <c r="K36" s="111"/>
-      <c r="L36" s="111"/>
-      <c r="M36" s="111"/>
-      <c r="N36" s="111"/>
-      <c r="O36" s="111"/>
-      <c r="P36" s="111"/>
-      <c r="Q36" s="116"/>
+        <v>15.676600000000001</v>
+      </c>
+      <c r="K36" s="123"/>
+      <c r="L36" s="123"/>
+      <c r="M36" s="123"/>
+      <c r="N36" s="123"/>
+      <c r="O36" s="123"/>
+      <c r="P36" s="123"/>
+      <c r="Q36" s="128"/>
       <c r="R36" s="42"/>
       <c r="S36" s="42"/>
       <c r="T36" s="42"/>
@@ -4285,7 +4282,7 @@
       <c r="AJ36" s="42"/>
       <c r="AK36" s="42"/>
     </row>
-    <row r="37" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -4299,7 +4296,7 @@
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -4313,7 +4310,7 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -4327,47 +4324,42 @@
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
     </row>
-    <row r="40" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
     </row>
-    <row r="46" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
     </row>
-    <row r="47" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
     </row>
-    <row r="48" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:37" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="6"/>
     </row>
-    <row r="53" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="6"/>
     </row>
-    <row r="54" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="6"/>
     </row>
-    <row r="55" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="6"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="B13:B18"/>
-    <mergeCell ref="C13:C18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
     <mergeCell ref="J2:Q2"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="H34:I34"/>
@@ -4380,6 +4372,11 @@
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="C27:C30"/>
     <mergeCell ref="J32:Q32"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="B13:B18"/>
+    <mergeCell ref="C13:C18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4388,31 +4385,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK82"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="43.6640625" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" customWidth="1"/>
-    <col min="4" max="4" width="55.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" customWidth="1"/>
-    <col min="15" max="15" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
+    <col min="4" max="4" width="55.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:37" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>20</v>
       </c>
@@ -4420,17 +4417,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J2" s="110" t="s">
+    <row r="2" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="112"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
+      <c r="Q2" s="124"/>
       <c r="R2" s="52"/>
       <c r="S2" s="42"/>
       <c r="T2" s="42"/>
@@ -4452,7 +4449,7 @@
       <c r="AJ2" s="42"/>
       <c r="AK2" s="42"/>
     </row>
-    <row r="3" spans="1:37" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
@@ -4522,8 +4519,8 @@
       <c r="AJ3" s="41"/>
       <c r="AK3" s="41"/>
     </row>
-    <row r="4" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="139" t="s">
+    <row r="4" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="149" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="66" t="s">
@@ -4567,8 +4564,8 @@
       <c r="AJ4" s="25"/>
       <c r="AK4" s="25"/>
     </row>
-    <row r="5" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="140"/>
+    <row r="5" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="150"/>
       <c r="C5" s="67" t="s">
         <v>24</v>
       </c>
@@ -4610,8 +4607,8 @@
       <c r="AJ5" s="25"/>
       <c r="AK5" s="25"/>
     </row>
-    <row r="6" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="140"/>
+    <row r="6" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="150"/>
       <c r="C6" s="56" t="s">
         <v>25</v>
       </c>
@@ -4653,8 +4650,8 @@
       <c r="AJ6" s="25"/>
       <c r="AK6" s="25"/>
     </row>
-    <row r="7" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="140"/>
+    <row r="7" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="150"/>
       <c r="C7" s="56" t="s">
         <v>26</v>
       </c>
@@ -4696,8 +4693,8 @@
       <c r="AJ7" s="25"/>
       <c r="AK7" s="25"/>
     </row>
-    <row r="8" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="140"/>
+    <row r="8" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="150"/>
       <c r="C8" s="56" t="s">
         <v>56</v>
       </c>
@@ -4736,8 +4733,8 @@
       <c r="AJ8" s="25"/>
       <c r="AK8" s="25"/>
     </row>
-    <row r="9" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="140"/>
+    <row r="9" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="150"/>
       <c r="C9" s="56" t="s">
         <v>55</v>
       </c>
@@ -4776,8 +4773,8 @@
       <c r="AJ9" s="25"/>
       <c r="AK9" s="25"/>
     </row>
-    <row r="10" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="140"/>
+    <row r="10" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="150"/>
       <c r="C10" s="56" t="s">
         <v>27</v>
       </c>
@@ -4819,8 +4816,8 @@
       <c r="AJ10" s="25"/>
       <c r="AK10" s="25"/>
     </row>
-    <row r="11" spans="1:37" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="140"/>
+    <row r="11" spans="1:37" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="150"/>
       <c r="C11" s="56" t="s">
         <v>52</v>
       </c>
@@ -4862,8 +4859,8 @@
       <c r="AJ11" s="25"/>
       <c r="AK11" s="25"/>
     </row>
-    <row r="12" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="141" t="s">
+    <row r="12" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="151" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="56" t="s">
@@ -4907,8 +4904,8 @@
       <c r="AJ12" s="25"/>
       <c r="AK12" s="25"/>
     </row>
-    <row r="13" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="142"/>
+    <row r="13" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="152"/>
       <c r="C13" s="56" t="s">
         <v>31</v>
       </c>
@@ -4950,8 +4947,8 @@
       <c r="AJ13" s="25"/>
       <c r="AK13" s="25"/>
     </row>
-    <row r="14" spans="1:37" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="142"/>
+    <row r="14" spans="1:37" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="152"/>
       <c r="C14" s="56" t="s">
         <v>30</v>
       </c>
@@ -4993,8 +4990,8 @@
       <c r="AJ14" s="25"/>
       <c r="AK14" s="25"/>
     </row>
-    <row r="15" spans="1:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="143"/>
+    <row r="15" spans="1:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="153"/>
       <c r="C15" s="56" t="s">
         <v>32</v>
       </c>
@@ -5036,11 +5033,11 @@
       <c r="AJ15" s="25"/>
       <c r="AK15" s="37"/>
     </row>
-    <row r="16" spans="1:37" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="144" t="s">
+    <row r="16" spans="1:37" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="154" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="147" t="s">
+      <c r="C16" s="157" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="25" t="s">
@@ -5083,9 +5080,9 @@
       <c r="AJ16" s="25"/>
       <c r="AK16" s="25"/>
     </row>
-    <row r="17" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="145"/>
-      <c r="C17" s="148"/>
+    <row r="17" spans="2:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="155"/>
+      <c r="C17" s="158"/>
       <c r="D17" s="25" t="s">
         <v>36</v>
       </c>
@@ -5126,9 +5123,9 @@
       <c r="AJ17" s="25"/>
       <c r="AK17" s="25"/>
     </row>
-    <row r="18" spans="2:37" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="145"/>
-      <c r="C18" s="149"/>
+    <row r="18" spans="2:37" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="155"/>
+      <c r="C18" s="159"/>
       <c r="D18" s="25" t="s">
         <v>37</v>
       </c>
@@ -5169,8 +5166,8 @@
       <c r="AJ18" s="25"/>
       <c r="AK18" s="25"/>
     </row>
-    <row r="19" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="145"/>
+    <row r="19" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="155"/>
       <c r="C19" s="62"/>
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
@@ -5210,8 +5207,8 @@
       <c r="AJ19" s="25"/>
       <c r="AK19" s="25"/>
     </row>
-    <row r="20" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="145"/>
+    <row r="20" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="155"/>
       <c r="C20" s="62"/>
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
@@ -5251,8 +5248,8 @@
       <c r="AJ20" s="25"/>
       <c r="AK20" s="25"/>
     </row>
-    <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="145"/>
+    <row r="21" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="155"/>
       <c r="C21" s="62"/>
       <c r="D21" s="25"/>
       <c r="E21" s="25"/>
@@ -5292,8 +5289,8 @@
       <c r="AJ21" s="25"/>
       <c r="AK21" s="25"/>
     </row>
-    <row r="22" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="146"/>
+    <row r="22" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="156"/>
       <c r="C22" s="62"/>
       <c r="D22" s="25"/>
       <c r="E22" s="25"/>
@@ -5333,7 +5330,7 @@
       <c r="AJ22" s="25"/>
       <c r="AK22" s="25"/>
     </row>
-    <row r="23" spans="2:37" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:37" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="34" t="s">
         <v>38</v>
       </c>
@@ -5378,11 +5375,11 @@
       <c r="AJ23" s="25"/>
       <c r="AK23" s="25"/>
     </row>
-    <row r="24" spans="2:37" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="135" t="s">
+    <row r="24" spans="2:37" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="137" t="s">
+      <c r="C24" s="144" t="s">
         <v>35</v>
       </c>
       <c r="D24" s="25" t="s">
@@ -5425,9 +5422,9 @@
       <c r="AJ24" s="37"/>
       <c r="AK24" s="25"/>
     </row>
-    <row r="25" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="126"/>
-      <c r="C25" s="133"/>
+    <row r="25" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="117"/>
+      <c r="C25" s="120"/>
       <c r="D25" s="25" t="s">
         <v>41</v>
       </c>
@@ -5468,9 +5465,9 @@
       <c r="AJ25" s="37"/>
       <c r="AK25" s="25"/>
     </row>
-    <row r="26" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="136"/>
-      <c r="C26" s="138"/>
+    <row r="26" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="143"/>
+      <c r="C26" s="145"/>
       <c r="D26" s="25" t="s">
         <v>48</v>
       </c>
@@ -5511,8 +5508,8 @@
       <c r="AJ26" s="37"/>
       <c r="AK26" s="25"/>
     </row>
-    <row r="27" spans="2:37" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="135" t="s">
+    <row r="27" spans="2:37" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="142" t="s">
         <v>42</v>
       </c>
       <c r="C27" s="69" t="s">
@@ -5556,8 +5553,8 @@
       <c r="AJ27" s="37"/>
       <c r="AK27" s="25"/>
     </row>
-    <row r="28" spans="2:37" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="126"/>
+    <row r="28" spans="2:37" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="117"/>
       <c r="C28" s="64" t="s">
         <v>54</v>
       </c>
@@ -5596,8 +5593,8 @@
       <c r="AJ28" s="37"/>
       <c r="AK28" s="25"/>
     </row>
-    <row r="29" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="126"/>
+    <row r="29" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="117"/>
       <c r="C29" s="68" t="s">
         <v>44</v>
       </c>
@@ -5639,8 +5636,8 @@
       <c r="AJ29" s="38"/>
       <c r="AK29" s="37"/>
     </row>
-    <row r="30" spans="2:37" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="136"/>
+    <row r="30" spans="2:37" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="143"/>
       <c r="C30" s="63" t="s">
         <v>53</v>
       </c>
@@ -5682,11 +5679,11 @@
       <c r="AJ30" s="37"/>
       <c r="AK30" s="37"/>
     </row>
-    <row r="31" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="135" t="s">
+    <row r="31" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="142" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="137" t="s">
+      <c r="C31" s="144" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="25" t="s">
@@ -5729,9 +5726,9 @@
       <c r="AJ31" s="37"/>
       <c r="AK31" s="37"/>
     </row>
-    <row r="32" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="126"/>
-      <c r="C32" s="133"/>
+    <row r="32" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="117"/>
+      <c r="C32" s="120"/>
       <c r="D32" s="25" t="s">
         <v>46</v>
       </c>
@@ -5772,9 +5769,9 @@
       <c r="AJ32" s="37"/>
       <c r="AK32" s="37"/>
     </row>
-    <row r="33" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="126"/>
-      <c r="C33" s="138"/>
+    <row r="33" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="117"/>
+      <c r="C33" s="145"/>
       <c r="D33" s="25" t="s">
         <v>47</v>
       </c>
@@ -5815,8 +5812,8 @@
       <c r="AJ33" s="37"/>
       <c r="AK33" s="37"/>
     </row>
-    <row r="34" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="136"/>
+    <row r="34" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="143"/>
       <c r="C34" s="63"/>
       <c r="D34" s="25"/>
       <c r="E34" s="25"/>
@@ -5856,8 +5853,8 @@
       <c r="AJ34" s="37"/>
       <c r="AK34" s="37"/>
     </row>
-    <row r="35" spans="2:37" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="135" t="s">
+    <row r="35" spans="2:37" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="142" t="s">
         <v>49</v>
       </c>
       <c r="C35" s="63" t="s">
@@ -5901,8 +5898,8 @@
       <c r="AJ35" s="37"/>
       <c r="AK35" s="37"/>
     </row>
-    <row r="36" spans="2:37" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="126"/>
+    <row r="36" spans="2:37" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="117"/>
       <c r="C36" s="58" t="s">
         <v>51</v>
       </c>
@@ -5944,8 +5941,8 @@
       <c r="AJ36" s="25"/>
       <c r="AK36" s="37"/>
     </row>
-    <row r="37" spans="2:37" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="126"/>
+    <row r="37" spans="2:37" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="117"/>
       <c r="C37" s="58"/>
       <c r="D37" s="25"/>
       <c r="E37" s="25"/>
@@ -5985,8 +5982,8 @@
       <c r="AJ37" s="25"/>
       <c r="AK37" s="37"/>
     </row>
-    <row r="38" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="136"/>
+    <row r="38" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="143"/>
       <c r="C38" s="54"/>
       <c r="D38" s="25"/>
       <c r="E38" s="25"/>
@@ -6026,7 +6023,7 @@
       <c r="AJ38" s="37"/>
       <c r="AK38" s="37"/>
     </row>
-    <row r="39" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="65"/>
       <c r="C39" s="58"/>
       <c r="D39" s="25"/>
@@ -6067,7 +6064,7 @@
       <c r="AJ39" s="38"/>
       <c r="AK39" s="37"/>
     </row>
-    <row r="40" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:37" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="65"/>
       <c r="C40" s="58"/>
       <c r="D40" s="25"/>
@@ -6108,7 +6105,7 @@
       <c r="AJ40" s="25"/>
       <c r="AK40" s="37"/>
     </row>
-    <row r="41" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="65"/>
       <c r="C41" s="58"/>
       <c r="D41" s="25"/>
@@ -6149,7 +6146,7 @@
       <c r="AJ41" s="25"/>
       <c r="AK41" s="37"/>
     </row>
-    <row r="42" spans="2:37" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:37" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="65"/>
       <c r="C42" s="58"/>
       <c r="D42" s="25"/>
@@ -6190,7 +6187,7 @@
       <c r="AJ42" s="25"/>
       <c r="AK42" s="37"/>
     </row>
-    <row r="43" spans="2:37" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:37" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="65"/>
       <c r="C43" s="58"/>
       <c r="D43" s="25"/>
@@ -6231,7 +6228,7 @@
       <c r="AJ43" s="25"/>
       <c r="AK43" s="37"/>
     </row>
-    <row r="44" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="65"/>
       <c r="C44" s="58"/>
       <c r="D44" s="25"/>
@@ -6272,7 +6269,7 @@
       <c r="AJ44" s="25"/>
       <c r="AK44" s="37"/>
     </row>
-    <row r="45" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="65"/>
       <c r="C45" s="64"/>
       <c r="D45" s="25"/>
@@ -6313,7 +6310,7 @@
       <c r="AJ45" s="38"/>
       <c r="AK45" s="38"/>
     </row>
-    <row r="46" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="65"/>
       <c r="C46" s="64"/>
       <c r="D46" s="25"/>
@@ -6354,7 +6351,7 @@
       <c r="AJ46" s="38"/>
       <c r="AK46" s="38"/>
     </row>
-    <row r="47" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B47" s="65"/>
       <c r="C47" s="55"/>
       <c r="D47" s="25"/>
@@ -6395,7 +6392,7 @@
       <c r="AJ47" s="25"/>
       <c r="AK47" s="37"/>
     </row>
-    <row r="48" spans="2:37" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:37" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="65"/>
       <c r="C48" s="58"/>
       <c r="D48" s="25"/>
@@ -6436,8 +6433,8 @@
       <c r="AJ48" s="37"/>
       <c r="AK48" s="37"/>
     </row>
-    <row r="49" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="152"/>
+    <row r="49" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="146"/>
       <c r="C49" s="37"/>
       <c r="D49" s="25"/>
       <c r="E49" s="37"/>
@@ -6477,8 +6474,8 @@
       <c r="AJ49" s="25"/>
       <c r="AK49" s="25"/>
     </row>
-    <row r="50" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="152"/>
+    <row r="50" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="146"/>
       <c r="C50" s="37"/>
       <c r="D50" s="25"/>
       <c r="E50" s="37"/>
@@ -6518,8 +6515,8 @@
       <c r="AJ50" s="25"/>
       <c r="AK50" s="25"/>
     </row>
-    <row r="51" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="152"/>
+    <row r="51" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="146"/>
       <c r="C51" s="62"/>
       <c r="D51" s="25"/>
       <c r="E51" s="37"/>
@@ -6559,8 +6556,8 @@
       <c r="AJ51" s="25"/>
       <c r="AK51" s="25"/>
     </row>
-    <row r="52" spans="2:37" ht="21" x14ac:dyDescent="0.3">
-      <c r="B52" s="153"/>
+    <row r="52" spans="2:37" ht="21" x14ac:dyDescent="0.25">
+      <c r="B52" s="147"/>
       <c r="C52" s="62"/>
       <c r="D52" s="25"/>
       <c r="E52" s="37"/>
@@ -6600,8 +6597,8 @@
       <c r="AJ52" s="25"/>
       <c r="AK52" s="25"/>
     </row>
-    <row r="53" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="154"/>
+    <row r="53" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="148"/>
       <c r="C53" s="56"/>
       <c r="D53" s="25"/>
       <c r="E53" s="37"/>
@@ -6641,8 +6638,8 @@
       <c r="AJ53" s="25"/>
       <c r="AK53" s="25"/>
     </row>
-    <row r="54" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="154"/>
+    <row r="54" spans="2:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="148"/>
       <c r="C54" s="56"/>
       <c r="D54" s="25"/>
       <c r="E54" s="37"/>
@@ -6682,8 +6679,8 @@
       <c r="AJ54" s="25"/>
       <c r="AK54" s="25"/>
     </row>
-    <row r="55" spans="2:37" ht="21" x14ac:dyDescent="0.3">
-      <c r="B55" s="154"/>
+    <row r="55" spans="2:37" ht="21" x14ac:dyDescent="0.25">
+      <c r="B55" s="148"/>
       <c r="C55" s="37"/>
       <c r="D55" s="25"/>
       <c r="E55" s="37"/>
@@ -6723,8 +6720,8 @@
       <c r="AJ55" s="25"/>
       <c r="AK55" s="25"/>
     </row>
-    <row r="56" spans="2:37" ht="21" x14ac:dyDescent="0.3">
-      <c r="B56" s="154"/>
+    <row r="56" spans="2:37" ht="21" x14ac:dyDescent="0.25">
+      <c r="B56" s="148"/>
       <c r="C56" s="37"/>
       <c r="D56" s="25"/>
       <c r="E56" s="37"/>
@@ -6764,15 +6761,15 @@
       <c r="AJ56" s="38"/>
       <c r="AK56" s="38"/>
     </row>
-    <row r="57" spans="2:37" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="150" t="s">
+    <row r="57" spans="2:37" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="140" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="151"/>
-      <c r="D57" s="151"/>
-      <c r="E57" s="151"/>
-      <c r="F57" s="151"/>
-      <c r="G57" s="151"/>
+      <c r="C57" s="141"/>
+      <c r="D57" s="141"/>
+      <c r="E57" s="141"/>
+      <c r="F57" s="141"/>
+      <c r="G57" s="141"/>
       <c r="H57" s="60">
         <f t="shared" ref="H57:I57" si="2">SUM(H4:H56)</f>
         <v>0</v>
@@ -6810,7 +6807,7 @@
       <c r="AJ57" s="35"/>
       <c r="AK57" s="35"/>
     </row>
-    <row r="58" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -6850,7 +6847,7 @@
       <c r="AJ58" s="42"/>
       <c r="AK58" s="42"/>
     </row>
-    <row r="59" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="16" t="s">
         <v>19</v>
       </c>
@@ -6894,7 +6891,7 @@
       <c r="AJ59" s="45"/>
       <c r="AK59" s="45"/>
     </row>
-    <row r="60" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="22" t="s">
         <v>14</v>
       </c>
@@ -6903,10 +6900,10 @@
       <c r="E60" s="29"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
-      <c r="H60" s="110" t="s">
+      <c r="H60" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="I60" s="116"/>
+      <c r="I60" s="128"/>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
       <c r="L60" s="9"/>
@@ -6936,7 +6933,7 @@
       <c r="AJ60" s="35"/>
       <c r="AK60" s="35"/>
     </row>
-    <row r="61" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="20" t="s">
         <v>13</v>
       </c>
@@ -6972,7 +6969,7 @@
       <c r="AJ61" s="45"/>
       <c r="AK61" s="45"/>
     </row>
-    <row r="62" spans="2:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="20" t="s">
         <v>15</v>
       </c>
@@ -6980,21 +6977,21 @@
       <c r="D62" s="31"/>
       <c r="E62" s="32"/>
       <c r="F62" s="3"/>
-      <c r="H62" s="110" t="s">
+      <c r="H62" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="I62" s="111"/>
-      <c r="J62" s="110">
+      <c r="I62" s="123"/>
+      <c r="J62" s="122">
         <f>H57-I57</f>
         <v>0</v>
       </c>
-      <c r="K62" s="111"/>
-      <c r="L62" s="111"/>
-      <c r="M62" s="111"/>
-      <c r="N62" s="111"/>
-      <c r="O62" s="111"/>
-      <c r="P62" s="111"/>
-      <c r="Q62" s="116"/>
+      <c r="K62" s="123"/>
+      <c r="L62" s="123"/>
+      <c r="M62" s="123"/>
+      <c r="N62" s="123"/>
+      <c r="O62" s="123"/>
+      <c r="P62" s="123"/>
+      <c r="Q62" s="128"/>
       <c r="R62" s="42"/>
       <c r="S62" s="42"/>
       <c r="T62" s="42"/>
@@ -7016,7 +7013,7 @@
       <c r="AJ62" s="42"/>
       <c r="AK62" s="42"/>
     </row>
-    <row r="63" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -7030,7 +7027,7 @@
       <c r="L63" s="3"/>
       <c r="M63" s="3"/>
     </row>
-    <row r="64" spans="2:37" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -7044,7 +7041,7 @@
       <c r="L64" s="3"/>
       <c r="M64" s="3"/>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -7058,42 +7055,49 @@
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
     </row>
-    <row r="66" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="6"/>
     </row>
-    <row r="72" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
     </row>
-    <row r="73" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="6"/>
     </row>
-    <row r="74" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="6"/>
     </row>
-    <row r="79" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="6"/>
     </row>
-    <row r="80" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="6"/>
     </row>
-    <row r="81" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="6"/>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="J2:Q2"/>
+    <mergeCell ref="B4:B11"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="C16:C18"/>
     <mergeCell ref="B57:G57"/>
     <mergeCell ref="H60:I60"/>
     <mergeCell ref="H62:I62"/>
@@ -7104,13 +7108,6 @@
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="B49:B52"/>
     <mergeCell ref="B53:B56"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="J2:Q2"/>
-    <mergeCell ref="B4:B11"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="C16:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7118,12 +7115,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>